<commit_message>
Mail impeccable fin de journée 14 juin
</commit_message>
<xml_diff>
--- a/Planning d'intervention Maintenance POUR TESTS.xlsx
+++ b/Planning d'intervention Maintenance POUR TESTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1 Dossiers de Nicolas\Etudes EPF\Swish\Code\BotMail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FABC43A-B9FF-47B6-BCF4-6D629F71B644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AB710B-3FB0-443C-96EB-DA28825D36A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
   </bookViews>
@@ -1923,18 +1923,19 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="40.109375" customWidth="1"/>
@@ -8737,6 +8738,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E948A9CE1FB2CE4C8AE9B70A9B9CE023" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8a8860a1c4c91bbc706a6e17b12ecc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b78c6ca-c81e-4330-9bb3-0f577d436514" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33efc8288bb545af800450190bca8712" ns2:_="">
     <xsd:import namespace="6b78c6ca-c81e-4330-9bb3-0f577d436514"/>
@@ -8868,15 +8878,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8884,6 +8885,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E650D547-6807-4F22-A8C4-3B6D59729371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8901,14 +8910,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC99D9B8-395A-430E-937C-0EA8E9C71B29}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Changement Excel - armoires électriques
</commit_message>
<xml_diff>
--- a/Planning d'intervention Maintenance POUR TESTS.xlsx
+++ b/Planning d'intervention Maintenance POUR TESTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1 Dossiers de Nicolas\Etudes EPF\Swish\Code\BotMail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a490776a08fd031/Documents/EPF S6/Swish/BotMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D99371-975A-4B1B-A6E7-E7606522DF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{72D99371-975A-4B1B-A6E7-E7606522DF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94714DF9-A479-4964-A321-0CE8393BEC55}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16EB6ED4-2E25-4642-8164-370FEBA71D91}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="172">
   <si>
     <t>Entreprise</t>
   </si>
@@ -576,32 +576,10 @@
     <t>Bornes simples</t>
   </si>
   <si>
-    <r>
-      <t>1 armoire électrique</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1 armoire électrique  </t>
-  </si>
-  <si>
     <t>4 (Evlink Schneider paramétrables)</t>
   </si>
   <si>
     <t>4 (ALFEN EVE SINGLE PRO LINE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 armoire électrique </t>
   </si>
   <si>
     <t xml:space="preserve">4 (ALFEN EVE DOUBLE PRO LINE) </t>
@@ -647,16 +625,10 @@
     <t>OK</t>
   </si>
   <si>
-    <t>1 armoire électrique</t>
-  </si>
-  <si>
     <t>3 (ALFEN)</t>
   </si>
   <si>
     <t>2 (ALFEN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 armoires électriques </t>
   </si>
   <si>
     <t>10 (ALFEN)</t>
@@ -1316,55 +1288,7 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1483,29 +1407,77 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1682,7 +1654,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1983,31 +1955,31 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="40.109375" customWidth="1"/>
-    <col min="10" max="12" width="24.6640625" customWidth="1"/>
-    <col min="13" max="14" width="24.6640625" style="45" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" style="46" customWidth="1"/>
-    <col min="16" max="17" width="21.33203125" style="47" customWidth="1"/>
-    <col min="18" max="18" width="20.44140625" style="48" customWidth="1"/>
-    <col min="19" max="20" width="20.44140625" style="49" customWidth="1"/>
-    <col min="21" max="21" width="20.88671875" style="50" customWidth="1"/>
-    <col min="22" max="22" width="2.44140625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="40.140625" customWidth="1"/>
+    <col min="10" max="12" width="24.7109375" customWidth="1"/>
+    <col min="13" max="14" width="24.7109375" style="45" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" style="46" customWidth="1"/>
+    <col min="16" max="17" width="21.28515625" style="47" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" style="48" customWidth="1"/>
+    <col min="19" max="20" width="20.42578125" style="49" customWidth="1"/>
+    <col min="21" max="21" width="20.85546875" style="50" customWidth="1"/>
+    <col min="22" max="22" width="2.42578125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="9.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -2021,1554 +1993,1554 @@
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="73"/>
-    </row>
-    <row r="3" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="96" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="58"/>
+    </row>
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="81" t="s">
         <v>144</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="96" t="s">
+      <c r="G3" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="H3" s="96" t="s">
-        <v>172</v>
-      </c>
-      <c r="I3" s="96" t="s">
-        <v>173</v>
-      </c>
-      <c r="J3" s="97" t="s">
-        <v>176</v>
-      </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="L3" s="97" t="s">
-        <v>158</v>
-      </c>
-      <c r="M3" s="98" t="s">
-        <v>174</v>
-      </c>
-      <c r="N3" s="98" t="s">
-        <v>163</v>
-      </c>
-      <c r="O3" s="99" t="s">
+      <c r="L3" s="82" t="s">
+        <v>155</v>
+      </c>
+      <c r="M3" s="83" t="s">
+        <v>169</v>
+      </c>
+      <c r="N3" s="83" t="s">
+        <v>160</v>
+      </c>
+      <c r="O3" s="84" t="s">
         <v>137</v>
       </c>
-      <c r="P3" s="100" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q3" s="100" t="s">
-        <v>163</v>
-      </c>
-      <c r="R3" s="101" t="s">
+      <c r="P3" s="85" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q3" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="R3" s="86" t="s">
         <v>138</v>
       </c>
-      <c r="S3" s="102" t="s">
+      <c r="S3" s="87" t="s">
         <v>139</v>
       </c>
-      <c r="T3" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="U3" s="103" t="s">
+      <c r="T3" s="87" t="s">
+        <v>160</v>
+      </c>
+      <c r="U3" s="88" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="74" t="s">
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="75" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" s="76">
+      <c r="B4" s="59"/>
+      <c r="C4" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60">
         <v>1</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="F4" s="61">
+        <v>1</v>
+      </c>
+      <c r="G4" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="I4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="78">
+      <c r="J4" s="63">
         <v>44557</v>
       </c>
-      <c r="K4" s="78"/>
-      <c r="L4" s="77">
+      <c r="K4" s="63"/>
+      <c r="L4" s="62">
         <v>12</v>
       </c>
-      <c r="M4" s="79">
+      <c r="M4" s="64">
         <f t="shared" ref="M4:M9" si="0">DATE(YEAR(J4)+1,MONTH(J4),DAY(J4))</f>
         <v>44922</v>
       </c>
-      <c r="N4" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="O4" s="80">
+      <c r="N4" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="65">
         <v>44922</v>
       </c>
-      <c r="P4" s="81">
+      <c r="P4" s="66">
         <f t="shared" ref="P4:P32" si="1">DATE(YEAR(J4)+2,MONTH(J4),DAY(J4))</f>
         <v>45287</v>
       </c>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="83">
+      <c r="Q4" s="66"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="68">
         <f t="shared" ref="S4:S32" si="2">DATE(YEAR(J4)+3,MONTH(J4),DAY(J4))</f>
         <v>45653</v>
       </c>
-      <c r="T4" s="83"/>
-      <c r="U4" s="84"/>
-    </row>
-    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="74" t="s">
+      <c r="T4" s="68"/>
+      <c r="U4" s="69"/>
+    </row>
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75" t="s">
+      <c r="B5" s="59"/>
+      <c r="C5" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60">
+        <v>1</v>
+      </c>
+      <c r="F5" s="61">
+        <v>1</v>
+      </c>
+      <c r="G5" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="63">
+        <v>44623</v>
+      </c>
+      <c r="K5" s="63"/>
+      <c r="L5" s="62">
+        <v>12</v>
+      </c>
+      <c r="M5" s="64">
+        <f t="shared" si="0"/>
+        <v>44988</v>
+      </c>
+      <c r="N5" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="O5" s="65">
+        <v>45034</v>
+      </c>
+      <c r="P5" s="66">
+        <f t="shared" si="1"/>
+        <v>45354</v>
+      </c>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="68">
+        <f t="shared" si="2"/>
+        <v>45719</v>
+      </c>
+      <c r="T5" s="68"/>
+      <c r="U5" s="69"/>
+    </row>
+    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="60">
+        <v>1</v>
+      </c>
+      <c r="F6" s="61">
+        <v>4</v>
+      </c>
+      <c r="G6" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="63">
+        <v>44743</v>
+      </c>
+      <c r="K6" s="63"/>
+      <c r="L6" s="62">
+        <v>12</v>
+      </c>
+      <c r="M6" s="64">
+        <f t="shared" si="0"/>
+        <v>45108</v>
+      </c>
+      <c r="N6" s="64"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="66">
+        <f t="shared" si="1"/>
+        <v>45474</v>
+      </c>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="68">
+        <f t="shared" si="2"/>
+        <v>45839</v>
+      </c>
+      <c r="T6" s="68"/>
+      <c r="U6" s="69"/>
+    </row>
+    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="76">
+      <c r="D7" s="60"/>
+      <c r="E7" s="60">
         <v>1</v>
       </c>
-      <c r="G5" s="77" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="77" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="77" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="78">
-        <v>44623</v>
-      </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="77">
+      <c r="F7" s="61">
+        <v>2</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="79">
-        <f t="shared" si="0"/>
-        <v>44988</v>
-      </c>
-      <c r="N5" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="O5" s="80">
-        <v>45034</v>
-      </c>
-      <c r="P5" s="81">
-        <f t="shared" si="1"/>
-        <v>45354</v>
-      </c>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="83">
-        <f t="shared" si="2"/>
-        <v>45719</v>
-      </c>
-      <c r="T5" s="83"/>
-      <c r="U5" s="84"/>
-    </row>
-    <row r="6" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="74" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="75" t="s">
+      <c r="J7" s="63">
+        <v>44668</v>
+      </c>
+      <c r="K7" s="63"/>
+      <c r="L7" s="62">
+        <v>12</v>
+      </c>
+      <c r="M7" s="64">
+        <f t="shared" si="0"/>
+        <v>45033</v>
+      </c>
+      <c r="N7" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="O7" s="65">
+        <v>45015</v>
+      </c>
+      <c r="P7" s="66">
+        <f t="shared" si="1"/>
+        <v>45399</v>
+      </c>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="68">
+        <f t="shared" si="2"/>
+        <v>45764</v>
+      </c>
+      <c r="T7" s="68"/>
+      <c r="U7" s="69"/>
+    </row>
+    <row r="8" spans="1:21" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61">
+        <v>1</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="63">
+        <v>44712</v>
+      </c>
+      <c r="K8" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="62">
+        <v>12</v>
+      </c>
+      <c r="M8" s="64">
+        <f t="shared" si="0"/>
+        <v>45077</v>
+      </c>
+      <c r="N8" s="64"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="66">
+        <f t="shared" si="1"/>
+        <v>45443</v>
+      </c>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="68">
+        <f t="shared" si="2"/>
+        <v>45808</v>
+      </c>
+      <c r="T8" s="68"/>
+      <c r="U8" s="69"/>
+    </row>
+    <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61">
+        <v>2</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="63">
+        <v>44747</v>
+      </c>
+      <c r="K9" s="63"/>
+      <c r="L9" s="62">
+        <v>12</v>
+      </c>
+      <c r="M9" s="64">
+        <f t="shared" si="0"/>
+        <v>45112</v>
+      </c>
+      <c r="N9" s="64"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="66">
+        <f t="shared" si="1"/>
+        <v>45478</v>
+      </c>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="68">
+        <f t="shared" si="2"/>
+        <v>45843</v>
+      </c>
+      <c r="T9" s="68"/>
+      <c r="U9" s="69"/>
+    </row>
+    <row r="10" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="75" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="F6" s="76">
-        <v>4</v>
-      </c>
-      <c r="G6" s="77" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="77" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="78">
-        <v>44743</v>
-      </c>
-      <c r="K6" s="78"/>
-      <c r="L6" s="77">
+      <c r="E10" s="60"/>
+      <c r="F10" s="61">
+        <v>1</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="62">
         <v>12</v>
       </c>
-      <c r="M6" s="79">
-        <f t="shared" si="0"/>
-        <v>45108</v>
-      </c>
-      <c r="N6" s="79"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="81">
-        <f t="shared" si="1"/>
-        <v>45474</v>
-      </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="83">
-        <f t="shared" si="2"/>
-        <v>45839</v>
-      </c>
-      <c r="T6" s="83"/>
-      <c r="U6" s="84"/>
-    </row>
-    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75" t="s">
-        <v>152</v>
-      </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="F7" s="76">
-        <v>2</v>
-      </c>
-      <c r="G7" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="78">
-        <v>44668</v>
-      </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="77">
-        <v>12</v>
-      </c>
-      <c r="M7" s="79">
-        <f t="shared" si="0"/>
-        <v>45033</v>
-      </c>
-      <c r="N7" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="O7" s="80">
-        <v>45015</v>
-      </c>
-      <c r="P7" s="81">
-        <f t="shared" si="1"/>
-        <v>45399</v>
-      </c>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="82"/>
-      <c r="S7" s="83">
-        <f t="shared" si="2"/>
-        <v>45764</v>
-      </c>
-      <c r="T7" s="83"/>
-      <c r="U7" s="84"/>
-    </row>
-    <row r="8" spans="1:21" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="76">
-        <v>1</v>
-      </c>
-      <c r="G8" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="78">
-        <v>44712</v>
-      </c>
-      <c r="K8" s="85" t="s">
-        <v>142</v>
-      </c>
-      <c r="L8" s="77">
-        <v>12</v>
-      </c>
-      <c r="M8" s="79">
-        <f t="shared" si="0"/>
-        <v>45077</v>
-      </c>
-      <c r="N8" s="79"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="81">
-        <f t="shared" si="1"/>
-        <v>45443</v>
-      </c>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="82"/>
-      <c r="S8" s="83">
-        <f t="shared" si="2"/>
-        <v>45808</v>
-      </c>
-      <c r="T8" s="83"/>
-      <c r="U8" s="84"/>
-    </row>
-    <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="76">
-        <v>2</v>
-      </c>
-      <c r="G9" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="77" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="78">
-        <v>44747</v>
-      </c>
-      <c r="K9" s="78"/>
-      <c r="L9" s="77">
-        <v>12</v>
-      </c>
-      <c r="M9" s="79">
-        <f t="shared" si="0"/>
-        <v>45112</v>
-      </c>
-      <c r="N9" s="79"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="81">
-        <f t="shared" si="1"/>
-        <v>45478</v>
-      </c>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="83">
-        <f t="shared" si="2"/>
-        <v>45843</v>
-      </c>
-      <c r="T9" s="83"/>
-      <c r="U9" s="84"/>
-    </row>
-    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="74" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" s="75"/>
-      <c r="F10" s="76">
-        <v>1</v>
-      </c>
-      <c r="G10" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="77" t="s">
-        <v>112</v>
-      </c>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="77">
-        <v>12</v>
-      </c>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="80" t="str">
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="65" t="str">
         <f>IF(J10="","",DATE(YEAR(J10)+1,MONTH(J10),DAY(J10)))</f>
         <v/>
       </c>
-      <c r="P10" s="81">
+      <c r="P10" s="66">
         <f t="shared" si="1"/>
         <v>731</v>
       </c>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="82" t="str">
+      <c r="Q10" s="66"/>
+      <c r="R10" s="67" t="str">
         <f>IF(J10="","",DATE(YEAR(O10)+1,MONTH(O10),DAY(O10)))</f>
         <v/>
       </c>
-      <c r="S10" s="83">
+      <c r="S10" s="68">
         <f t="shared" si="2"/>
         <v>1096</v>
       </c>
-      <c r="T10" s="83"/>
-      <c r="U10" s="84" t="str">
+      <c r="T10" s="68"/>
+      <c r="U10" s="69" t="str">
         <f>IF(J10="","",DATE(YEAR(R10)+1,MONTH(R10),DAY(R10)))</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="74" t="s">
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76">
+      <c r="B11" s="59"/>
+      <c r="C11" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61">
         <v>1</v>
       </c>
-      <c r="G11" s="77" t="s">
+      <c r="G11" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="77" t="s">
+      <c r="I11" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="78">
+      <c r="J11" s="63">
         <v>44704</v>
       </c>
-      <c r="K11" s="86"/>
-      <c r="L11" s="77">
+      <c r="K11" s="71"/>
+      <c r="L11" s="62">
         <v>12</v>
       </c>
-      <c r="M11" s="79">
+      <c r="M11" s="64">
         <f t="shared" ref="M11:M32" si="3">DATE(YEAR(J11)+1,MONTH(J11),DAY(J11))</f>
         <v>45069</v>
       </c>
-      <c r="N11" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="O11" s="80">
+      <c r="N11" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="O11" s="65">
         <v>45077</v>
       </c>
-      <c r="P11" s="81">
+      <c r="P11" s="66">
         <f t="shared" si="1"/>
         <v>45435</v>
       </c>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="82"/>
-      <c r="S11" s="83">
+      <c r="Q11" s="66"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="68">
         <f t="shared" si="2"/>
         <v>45800</v>
       </c>
-      <c r="T11" s="83"/>
-      <c r="U11" s="84"/>
-    </row>
-    <row r="12" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="74" t="s">
+      <c r="T11" s="68"/>
+      <c r="U11" s="69"/>
+    </row>
+    <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60">
+        <v>1</v>
+      </c>
+      <c r="F12" s="61">
+        <v>2</v>
+      </c>
+      <c r="G12" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="63">
+        <v>44726</v>
+      </c>
+      <c r="K12" s="63"/>
+      <c r="L12" s="62">
+        <v>12</v>
+      </c>
+      <c r="M12" s="64">
+        <f t="shared" si="3"/>
+        <v>45091</v>
+      </c>
+      <c r="N12" s="64"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="66">
+        <f t="shared" si="1"/>
+        <v>45457</v>
+      </c>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="68">
+        <f t="shared" si="2"/>
+        <v>45822</v>
+      </c>
+      <c r="T12" s="68"/>
+      <c r="U12" s="69"/>
+    </row>
+    <row r="13" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="60">
+        <v>1</v>
+      </c>
+      <c r="F13" s="61">
+        <v>2</v>
+      </c>
+      <c r="G13" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="63">
+        <v>44869</v>
+      </c>
+      <c r="K13" s="63"/>
+      <c r="L13" s="62">
+        <v>12</v>
+      </c>
+      <c r="M13" s="64">
+        <f t="shared" si="3"/>
+        <v>45234</v>
+      </c>
+      <c r="N13" s="64"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="66">
+        <f t="shared" si="1"/>
+        <v>45600</v>
+      </c>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="68">
+        <f t="shared" si="2"/>
+        <v>45965</v>
+      </c>
+      <c r="T13" s="68"/>
+      <c r="U13" s="69"/>
+    </row>
+    <row r="14" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" s="76">
+      <c r="D14" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="61">
         <v>2</v>
       </c>
-      <c r="G12" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="77" t="s">
+      <c r="G14" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="63">
+        <v>44839</v>
+      </c>
+      <c r="K14" s="63"/>
+      <c r="L14" s="62">
         <v>12</v>
       </c>
-      <c r="J12" s="78">
-        <v>44726</v>
-      </c>
-      <c r="K12" s="78"/>
-      <c r="L12" s="77">
+      <c r="M14" s="64">
+        <f t="shared" si="3"/>
+        <v>45204</v>
+      </c>
+      <c r="N14" s="64"/>
+      <c r="O14" s="65"/>
+      <c r="P14" s="66">
+        <f t="shared" si="1"/>
+        <v>45570</v>
+      </c>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="67"/>
+      <c r="S14" s="68">
+        <f t="shared" si="2"/>
+        <v>45935</v>
+      </c>
+      <c r="T14" s="68"/>
+      <c r="U14" s="69"/>
+    </row>
+    <row r="15" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="61">
+        <v>1</v>
+      </c>
+      <c r="G15" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="63">
+        <v>44799</v>
+      </c>
+      <c r="K15" s="63"/>
+      <c r="L15" s="62">
         <v>12</v>
       </c>
-      <c r="M12" s="79">
-        <f t="shared" si="3"/>
-        <v>45091</v>
-      </c>
-      <c r="N12" s="79"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="81">
-        <f t="shared" si="1"/>
-        <v>45457</v>
-      </c>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="82"/>
-      <c r="S12" s="83">
-        <f t="shared" si="2"/>
-        <v>45822</v>
-      </c>
-      <c r="T12" s="83"/>
-      <c r="U12" s="84"/>
-    </row>
-    <row r="13" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="F13" s="76">
-        <v>2</v>
-      </c>
-      <c r="G13" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="78">
-        <v>44869</v>
-      </c>
-      <c r="K13" s="78"/>
-      <c r="L13" s="77">
+      <c r="M15" s="64">
+        <f t="shared" si="3"/>
+        <v>45164</v>
+      </c>
+      <c r="N15" s="64"/>
+      <c r="O15" s="65"/>
+      <c r="P15" s="66">
+        <f t="shared" si="1"/>
+        <v>45530</v>
+      </c>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="67"/>
+      <c r="S15" s="68">
+        <f t="shared" si="2"/>
+        <v>45895</v>
+      </c>
+      <c r="T15" s="68"/>
+      <c r="U15" s="69"/>
+    </row>
+    <row r="16" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="61">
+        <v>1</v>
+      </c>
+      <c r="G16" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="63">
+        <v>44806</v>
+      </c>
+      <c r="K16" s="63"/>
+      <c r="L16" s="62">
         <v>12</v>
       </c>
-      <c r="M13" s="79">
-        <f t="shared" si="3"/>
-        <v>45234</v>
-      </c>
-      <c r="N13" s="79"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="81">
-        <f t="shared" si="1"/>
-        <v>45600</v>
-      </c>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="83">
-        <f t="shared" si="2"/>
-        <v>45965</v>
-      </c>
-      <c r="T13" s="83"/>
-      <c r="U13" s="84"/>
-    </row>
-    <row r="14" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="75" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14" s="76">
-        <v>2</v>
-      </c>
-      <c r="G14" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="78">
-        <v>44839</v>
-      </c>
-      <c r="K14" s="78"/>
-      <c r="L14" s="77">
+      <c r="M16" s="64">
+        <f t="shared" si="3"/>
+        <v>45171</v>
+      </c>
+      <c r="N16" s="64"/>
+      <c r="O16" s="65"/>
+      <c r="P16" s="66">
+        <f t="shared" si="1"/>
+        <v>45537</v>
+      </c>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="67"/>
+      <c r="S16" s="68">
+        <f t="shared" si="2"/>
+        <v>45902</v>
+      </c>
+      <c r="T16" s="68"/>
+      <c r="U16" s="69"/>
+    </row>
+    <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="60"/>
+      <c r="F17" s="61">
+        <v>1</v>
+      </c>
+      <c r="G17" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="63">
+        <v>44851</v>
+      </c>
+      <c r="K17" s="63"/>
+      <c r="L17" s="62">
         <v>12</v>
       </c>
-      <c r="M14" s="79">
-        <f t="shared" si="3"/>
-        <v>45204</v>
-      </c>
-      <c r="N14" s="79"/>
-      <c r="O14" s="80"/>
-      <c r="P14" s="81">
-        <f t="shared" si="1"/>
-        <v>45570</v>
-      </c>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="83">
-        <f t="shared" si="2"/>
-        <v>45935</v>
-      </c>
-      <c r="T14" s="83"/>
-      <c r="U14" s="84"/>
-    </row>
-    <row r="15" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="76">
+      <c r="M17" s="64">
+        <f t="shared" si="3"/>
+        <v>45216</v>
+      </c>
+      <c r="N17" s="64"/>
+      <c r="O17" s="65"/>
+      <c r="P17" s="66">
+        <f t="shared" si="1"/>
+        <v>45582</v>
+      </c>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="67"/>
+      <c r="S17" s="68">
+        <f t="shared" si="2"/>
+        <v>45947</v>
+      </c>
+      <c r="T17" s="68"/>
+      <c r="U17" s="69"/>
+    </row>
+    <row r="18" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="60"/>
+      <c r="F18" s="61">
         <v>1</v>
       </c>
-      <c r="G15" s="77" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="77" t="s">
+      <c r="G18" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="78">
-        <v>44799</v>
-      </c>
-      <c r="K15" s="78"/>
-      <c r="L15" s="77">
+      <c r="I18" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="63">
+        <v>44853</v>
+      </c>
+      <c r="K18" s="63"/>
+      <c r="L18" s="62">
         <v>12</v>
       </c>
-      <c r="M15" s="79">
-        <f t="shared" si="3"/>
-        <v>45164</v>
-      </c>
-      <c r="N15" s="79"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="81">
-        <f t="shared" si="1"/>
-        <v>45530</v>
-      </c>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="83">
-        <f t="shared" si="2"/>
-        <v>45895</v>
-      </c>
-      <c r="T15" s="83"/>
-      <c r="U15" s="84"/>
-    </row>
-    <row r="16" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="74"/>
-      <c r="C16" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="76">
+      <c r="M18" s="64">
+        <f t="shared" si="3"/>
+        <v>45218</v>
+      </c>
+      <c r="N18" s="64"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="66">
+        <f t="shared" si="1"/>
+        <v>45584</v>
+      </c>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="68">
+        <f t="shared" si="2"/>
+        <v>45949</v>
+      </c>
+      <c r="T18" s="68"/>
+      <c r="U18" s="69"/>
+    </row>
+    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="60"/>
+      <c r="F19" s="61">
         <v>1</v>
       </c>
-      <c r="G16" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="77" t="s">
+      <c r="G19" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="63">
+        <v>44875</v>
+      </c>
+      <c r="K19" s="63"/>
+      <c r="L19" s="62">
+        <v>12</v>
+      </c>
+      <c r="M19" s="64">
+        <f t="shared" si="3"/>
+        <v>45240</v>
+      </c>
+      <c r="N19" s="64"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="66">
+        <f t="shared" si="1"/>
+        <v>45606</v>
+      </c>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="68">
+        <f t="shared" si="2"/>
+        <v>45971</v>
+      </c>
+      <c r="T19" s="68"/>
+      <c r="U19" s="69"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61">
         <v>1</v>
       </c>
-      <c r="I16" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="78">
-        <v>44806</v>
-      </c>
-      <c r="K16" s="78"/>
-      <c r="L16" s="77">
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="62">
         <v>12</v>
       </c>
-      <c r="M16" s="79">
-        <f t="shared" si="3"/>
-        <v>45171</v>
-      </c>
-      <c r="N16" s="79"/>
-      <c r="O16" s="80"/>
-      <c r="P16" s="81">
-        <f t="shared" si="1"/>
-        <v>45537</v>
-      </c>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="82"/>
-      <c r="S16" s="83">
-        <f t="shared" si="2"/>
-        <v>45902</v>
-      </c>
-      <c r="T16" s="83"/>
-      <c r="U16" s="84"/>
-    </row>
-    <row r="17" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" s="75"/>
-      <c r="F17" s="76">
-        <v>1</v>
-      </c>
-      <c r="G17" s="77" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="77" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="77" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="78">
-        <v>44851</v>
-      </c>
-      <c r="K17" s="78"/>
-      <c r="L17" s="77">
-        <v>12</v>
-      </c>
-      <c r="M17" s="79">
-        <f t="shared" si="3"/>
-        <v>45216</v>
-      </c>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="81">
-        <f t="shared" si="1"/>
-        <v>45582</v>
-      </c>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="83">
-        <f t="shared" si="2"/>
-        <v>45947</v>
-      </c>
-      <c r="T17" s="83"/>
-      <c r="U17" s="84"/>
-    </row>
-    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="74" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="74"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="E18" s="75"/>
-      <c r="F18" s="76">
-        <v>1</v>
-      </c>
-      <c r="G18" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="77" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="J18" s="78">
-        <v>44853</v>
-      </c>
-      <c r="K18" s="78"/>
-      <c r="L18" s="77">
-        <v>12</v>
-      </c>
-      <c r="M18" s="79">
-        <f t="shared" si="3"/>
-        <v>45218</v>
-      </c>
-      <c r="N18" s="79"/>
-      <c r="O18" s="80"/>
-      <c r="P18" s="81">
-        <f t="shared" si="1"/>
-        <v>45584</v>
-      </c>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="83">
-        <f t="shared" si="2"/>
-        <v>45949</v>
-      </c>
-      <c r="T18" s="83"/>
-      <c r="U18" s="84"/>
-    </row>
-    <row r="19" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="76">
-        <v>1</v>
-      </c>
-      <c r="G19" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="77" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" s="78">
-        <v>44875</v>
-      </c>
-      <c r="K19" s="78"/>
-      <c r="L19" s="77">
-        <v>12</v>
-      </c>
-      <c r="M19" s="79">
-        <f t="shared" si="3"/>
-        <v>45240</v>
-      </c>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
-      <c r="P19" s="81">
-        <f t="shared" si="1"/>
-        <v>45606</v>
-      </c>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="82"/>
-      <c r="S19" s="83">
-        <f t="shared" si="2"/>
-        <v>45971</v>
-      </c>
-      <c r="T19" s="83"/>
-      <c r="U19" s="84"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="76">
-        <v>1</v>
-      </c>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="77">
-        <v>12</v>
-      </c>
-      <c r="M20" s="79">
+      <c r="M20" s="64">
         <f t="shared" si="3"/>
         <v>366</v>
       </c>
-      <c r="N20" s="79"/>
-      <c r="O20" s="80" t="str">
+      <c r="N20" s="64"/>
+      <c r="O20" s="65" t="str">
         <f>IF(J20="","",DATE(YEAR(J20)+1,MONTH(J20),DAY(J20)))</f>
         <v/>
       </c>
-      <c r="P20" s="81">
+      <c r="P20" s="66">
         <f t="shared" si="1"/>
         <v>731</v>
       </c>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="82" t="str">
+      <c r="Q20" s="66"/>
+      <c r="R20" s="67" t="str">
         <f>IF(J20="","",DATE(YEAR(O20)+1,MONTH(O20),DAY(O20)))</f>
         <v/>
       </c>
-      <c r="S20" s="83">
+      <c r="S20" s="68">
         <f t="shared" si="2"/>
         <v>1096</v>
       </c>
-      <c r="T20" s="83"/>
-      <c r="U20" s="84" t="str">
+      <c r="T20" s="68"/>
+      <c r="U20" s="69" t="str">
         <f>IF(J20="","",DATE(YEAR(R20)+1,MONTH(R20),DAY(R20)))</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="74" t="s">
+    <row r="21" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="76">
+      <c r="B21" s="59"/>
+      <c r="C21" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="61">
         <v>1</v>
       </c>
-      <c r="G21" s="77" t="s">
+      <c r="G21" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="H21" s="77" t="s">
+      <c r="H21" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="77" t="s">
+      <c r="I21" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="77">
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="62">
         <v>12</v>
       </c>
-      <c r="M21" s="79">
+      <c r="M21" s="64">
         <f t="shared" si="3"/>
         <v>366</v>
       </c>
-      <c r="N21" s="79"/>
-      <c r="O21" s="80" t="str">
+      <c r="N21" s="64"/>
+      <c r="O21" s="65" t="str">
         <f>IF(J21="","",DATE(YEAR(J21)+1,MONTH(J21),DAY(J21)))</f>
         <v/>
       </c>
-      <c r="P21" s="81">
+      <c r="P21" s="66">
         <f t="shared" si="1"/>
         <v>731</v>
       </c>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="82" t="str">
+      <c r="Q21" s="66"/>
+      <c r="R21" s="67" t="str">
         <f>IF(J21="","",DATE(YEAR(O21)+1,MONTH(O21),DAY(O21)))</f>
         <v/>
       </c>
-      <c r="S21" s="83">
+      <c r="S21" s="68">
         <f t="shared" si="2"/>
         <v>1096</v>
       </c>
-      <c r="T21" s="83"/>
-      <c r="U21" s="84" t="str">
+      <c r="T21" s="68"/>
+      <c r="U21" s="69" t="str">
         <f>IF(J21="","",DATE(YEAR(R21)+1,MONTH(R21),DAY(R21)))</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="74" t="s">
+    <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75" t="s">
+      <c r="B22" s="59"/>
+      <c r="C22" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="76">
+      <c r="D22" s="60"/>
+      <c r="E22" s="60">
+        <v>1</v>
+      </c>
+      <c r="F22" s="61">
         <v>4</v>
       </c>
-      <c r="G22" s="77" t="s">
+      <c r="G22" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="77" t="s">
+      <c r="H22" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="I22" s="77" t="s">
+      <c r="I22" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="77">
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="62">
         <v>12</v>
       </c>
-      <c r="M22" s="79">
+      <c r="M22" s="64">
         <f t="shared" si="3"/>
         <v>366</v>
       </c>
-      <c r="N22" s="79"/>
-      <c r="O22" s="80" t="str">
+      <c r="N22" s="64"/>
+      <c r="O22" s="65" t="str">
         <f>IF(J22="","",DATE(YEAR(J22)+1,MONTH(J22),DAY(J22)))</f>
         <v/>
       </c>
-      <c r="P22" s="81">
+      <c r="P22" s="66">
         <f t="shared" si="1"/>
         <v>731</v>
       </c>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="82" t="str">
+      <c r="Q22" s="66"/>
+      <c r="R22" s="67" t="str">
         <f>IF(J22="","",DATE(YEAR(O22)+1,MONTH(O22),DAY(O22)))</f>
         <v/>
       </c>
-      <c r="S22" s="83">
+      <c r="S22" s="68">
         <f t="shared" si="2"/>
         <v>1096</v>
       </c>
-      <c r="T22" s="83"/>
-      <c r="U22" s="84" t="str">
+      <c r="T22" s="68"/>
+      <c r="U22" s="69" t="str">
         <f>IF(J22="","",DATE(YEAR(R22)+1,MONTH(R22),DAY(R22)))</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="74" t="s">
+    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75" t="s">
-        <v>165</v>
-      </c>
-      <c r="F23" s="76">
+      <c r="B23" s="59"/>
+      <c r="C23" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60">
+        <v>1</v>
+      </c>
+      <c r="F23" s="61">
         <v>2</v>
       </c>
-      <c r="G23" s="77" t="s">
+      <c r="G23" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="H23" s="77" t="s">
+      <c r="H23" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="I23" s="77" t="s">
+      <c r="I23" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="J23" s="78">
+      <c r="J23" s="63">
         <v>44998</v>
       </c>
-      <c r="K23" s="78"/>
-      <c r="L23" s="77">
+      <c r="K23" s="63"/>
+      <c r="L23" s="62">
         <v>12</v>
       </c>
-      <c r="M23" s="79">
+      <c r="M23" s="64">
         <f t="shared" si="3"/>
         <v>45364</v>
       </c>
-      <c r="N23" s="79"/>
-      <c r="O23" s="80"/>
-      <c r="P23" s="81">
+      <c r="N23" s="64"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="66">
         <f t="shared" si="1"/>
         <v>45729</v>
       </c>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="83">
+      <c r="Q23" s="66"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="68">
         <f t="shared" si="2"/>
         <v>46094</v>
       </c>
-      <c r="T23" s="83"/>
-      <c r="U23" s="84"/>
-    </row>
-    <row r="24" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="74" t="s">
+      <c r="T23" s="68"/>
+      <c r="U23" s="69"/>
+    </row>
+    <row r="24" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="75">
+      <c r="B24" s="59"/>
+      <c r="C24" s="60">
         <v>5</v>
       </c>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="76">
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="61">
         <v>2</v>
       </c>
-      <c r="G24" s="77" t="s">
+      <c r="G24" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="I24" s="77" t="s">
+      <c r="I24" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="J24" s="78">
+      <c r="J24" s="63">
         <v>44903</v>
       </c>
-      <c r="K24" s="78"/>
-      <c r="L24" s="77">
+      <c r="K24" s="63"/>
+      <c r="L24" s="62">
         <v>12</v>
       </c>
-      <c r="M24" s="79">
+      <c r="M24" s="64">
         <f t="shared" si="3"/>
         <v>45268</v>
       </c>
-      <c r="N24" s="79"/>
-      <c r="O24" s="80"/>
-      <c r="P24" s="81">
+      <c r="N24" s="64"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="66">
         <f t="shared" si="1"/>
         <v>45634</v>
       </c>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="82"/>
-      <c r="S24" s="83">
+      <c r="Q24" s="66"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="68">
         <f t="shared" si="2"/>
         <v>45999</v>
       </c>
-      <c r="T24" s="83"/>
-      <c r="U24" s="84"/>
-    </row>
-    <row r="25" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="74" t="s">
+      <c r="T24" s="68"/>
+      <c r="U24" s="69"/>
+    </row>
+    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75">
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60">
         <v>5</v>
       </c>
-      <c r="E25" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="F25" s="76"/>
-      <c r="G25" s="77" t="s">
+      <c r="E25" s="60">
+        <v>2</v>
+      </c>
+      <c r="F25" s="61"/>
+      <c r="G25" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="H25" s="77" t="s">
+      <c r="H25" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I25" s="77" t="s">
+      <c r="I25" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="J25" s="78">
+      <c r="J25" s="63">
         <v>44980</v>
       </c>
-      <c r="K25" s="78"/>
-      <c r="L25" s="77">
+      <c r="K25" s="63"/>
+      <c r="L25" s="62">
         <v>12</v>
       </c>
-      <c r="M25" s="79">
+      <c r="M25" s="64">
         <f t="shared" si="3"/>
         <v>45345</v>
       </c>
-      <c r="N25" s="79"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="81">
+      <c r="N25" s="64"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="66">
         <f t="shared" si="1"/>
         <v>45711</v>
       </c>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="82"/>
-      <c r="S25" s="83">
+      <c r="Q25" s="66"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="68">
         <f t="shared" si="2"/>
         <v>46076</v>
       </c>
-      <c r="T25" s="83"/>
-      <c r="U25" s="84"/>
-    </row>
-    <row r="26" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="T25" s="68"/>
+      <c r="U25" s="69"/>
+    </row>
+    <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="76">
+      <c r="B26" s="59"/>
+      <c r="C26" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="61">
         <v>1</v>
       </c>
-      <c r="G26" s="77" t="s">
+      <c r="G26" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="H26" s="77" t="s">
+      <c r="H26" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="I26" s="77" t="s">
+      <c r="I26" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="78">
+      <c r="J26" s="63">
         <v>44999</v>
       </c>
-      <c r="K26" s="78"/>
-      <c r="L26" s="77">
+      <c r="K26" s="63"/>
+      <c r="L26" s="62">
         <v>12</v>
       </c>
-      <c r="M26" s="79">
+      <c r="M26" s="64">
         <f t="shared" si="3"/>
         <v>45365</v>
       </c>
-      <c r="N26" s="79"/>
-      <c r="O26" s="80"/>
-      <c r="P26" s="81">
+      <c r="N26" s="64"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="66">
         <f t="shared" si="1"/>
         <v>45730</v>
       </c>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="82"/>
-      <c r="S26" s="83">
+      <c r="Q26" s="66"/>
+      <c r="R26" s="67"/>
+      <c r="S26" s="68">
         <f t="shared" si="2"/>
         <v>46095</v>
       </c>
-      <c r="T26" s="83"/>
-      <c r="U26" s="84"/>
-    </row>
-    <row r="27" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="74" t="s">
+      <c r="T26" s="68"/>
+      <c r="U26" s="69"/>
+    </row>
+    <row r="27" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="76">
+      <c r="B27" s="59"/>
+      <c r="C27" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="61">
         <v>1</v>
       </c>
-      <c r="G27" s="77" t="s">
+      <c r="G27" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="77" t="s">
+      <c r="H27" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="I27" s="77" t="s">
+      <c r="I27" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="78">
+      <c r="J27" s="63">
         <v>44995</v>
       </c>
-      <c r="K27" s="78"/>
-      <c r="L27" s="77">
+      <c r="K27" s="63"/>
+      <c r="L27" s="62">
         <v>12</v>
       </c>
-      <c r="M27" s="79">
+      <c r="M27" s="64">
         <f t="shared" si="3"/>
         <v>45361</v>
       </c>
-      <c r="N27" s="79"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="81">
+      <c r="N27" s="64"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="66">
         <f t="shared" si="1"/>
         <v>45726</v>
       </c>
-      <c r="Q27" s="81"/>
-      <c r="R27" s="82"/>
-      <c r="S27" s="83">
+      <c r="Q27" s="66"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="68">
         <f t="shared" si="2"/>
         <v>46091</v>
       </c>
-      <c r="T27" s="83"/>
-      <c r="U27" s="84"/>
-    </row>
-    <row r="28" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="74" t="s">
+      <c r="T27" s="68"/>
+      <c r="U27" s="69"/>
+    </row>
+    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="76">
+      <c r="B28" s="59"/>
+      <c r="C28" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="61">
         <v>1</v>
       </c>
-      <c r="G28" s="77" t="s">
+      <c r="G28" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="H28" s="77" t="s">
+      <c r="H28" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="I28" s="77" t="s">
+      <c r="I28" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="78">
+      <c r="J28" s="63">
         <v>44993</v>
       </c>
-      <c r="K28" s="78"/>
-      <c r="L28" s="77">
+      <c r="K28" s="63"/>
+      <c r="L28" s="62">
         <v>12</v>
       </c>
-      <c r="M28" s="79">
+      <c r="M28" s="64">
         <f t="shared" si="3"/>
         <v>45359</v>
       </c>
-      <c r="N28" s="79"/>
-      <c r="O28" s="80"/>
-      <c r="P28" s="81">
+      <c r="N28" s="64"/>
+      <c r="O28" s="65"/>
+      <c r="P28" s="66">
         <f t="shared" si="1"/>
         <v>45724</v>
       </c>
-      <c r="Q28" s="81"/>
-      <c r="R28" s="82"/>
-      <c r="S28" s="83">
+      <c r="Q28" s="66"/>
+      <c r="R28" s="67"/>
+      <c r="S28" s="68">
         <f t="shared" si="2"/>
         <v>46089</v>
       </c>
-      <c r="T28" s="83"/>
-      <c r="U28" s="84"/>
-    </row>
-    <row r="29" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="87" t="s">
+      <c r="T28" s="68"/>
+      <c r="U28" s="69"/>
+    </row>
+    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="B29" s="88"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75">
+      <c r="B29" s="73"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60">
         <v>5</v>
       </c>
-      <c r="E29" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="F29" s="88"/>
-      <c r="G29" s="89" t="s">
+      <c r="E29" s="60">
+        <v>1</v>
+      </c>
+      <c r="F29" s="73"/>
+      <c r="G29" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="H29" s="90" t="s">
+      <c r="H29" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="I29" s="89" t="s">
+      <c r="I29" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="J29" s="91">
+      <c r="J29" s="76">
         <v>45009</v>
       </c>
-      <c r="K29" s="78"/>
-      <c r="L29" s="77">
+      <c r="K29" s="63"/>
+      <c r="L29" s="62">
         <v>12</v>
       </c>
-      <c r="M29" s="79">
+      <c r="M29" s="64">
         <f t="shared" si="3"/>
         <v>45375</v>
       </c>
-      <c r="N29" s="79"/>
-      <c r="O29" s="80"/>
-      <c r="P29" s="81">
+      <c r="N29" s="64"/>
+      <c r="O29" s="65"/>
+      <c r="P29" s="66">
         <f t="shared" si="1"/>
         <v>45740</v>
       </c>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="82"/>
-      <c r="S29" s="83">
+      <c r="Q29" s="66"/>
+      <c r="R29" s="67"/>
+      <c r="S29" s="68">
         <f t="shared" si="2"/>
         <v>46105</v>
       </c>
-      <c r="T29" s="83"/>
-      <c r="U29" s="84"/>
-    </row>
-    <row r="30" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="87" cm="1">
+      <c r="T29" s="68"/>
+      <c r="U29" s="69"/>
+    </row>
+    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" cm="1">
         <f t="array" aca="1" ref="A30" ca="1">+E31+A30:O31+A30:U36</f>
         <v>0</v>
       </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="92">
+      <c r="B30" s="73"/>
+      <c r="C30" s="77">
         <v>1</v>
       </c>
-      <c r="D30" s="92">
+      <c r="D30" s="77">
         <v>5</v>
       </c>
-      <c r="E30" s="92" t="s">
-        <v>165</v>
-      </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89" t="s">
+      <c r="E30" s="77">
+        <v>1</v>
+      </c>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="H30" s="77" t="s">
+      <c r="H30" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I30" s="77" t="s">
+      <c r="I30" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="J30" s="91">
+      <c r="J30" s="76">
         <v>44964</v>
       </c>
-      <c r="K30" s="78"/>
-      <c r="L30" s="77">
+      <c r="K30" s="63"/>
+      <c r="L30" s="62">
         <v>12</v>
       </c>
-      <c r="M30" s="79">
+      <c r="M30" s="64">
         <f t="shared" si="3"/>
         <v>45329</v>
       </c>
-      <c r="N30" s="79"/>
-      <c r="O30" s="93"/>
-      <c r="P30" s="81">
+      <c r="N30" s="64"/>
+      <c r="O30" s="78"/>
+      <c r="P30" s="66">
         <f t="shared" si="1"/>
         <v>45695</v>
       </c>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="94"/>
-      <c r="S30" s="83">
+      <c r="Q30" s="66"/>
+      <c r="R30" s="79"/>
+      <c r="S30" s="68">
         <f t="shared" si="2"/>
         <v>46060</v>
       </c>
-      <c r="T30" s="83"/>
-      <c r="U30" s="95"/>
-    </row>
-    <row r="31" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="87" t="s">
+      <c r="T30" s="68"/>
+      <c r="U30" s="80"/>
+    </row>
+    <row r="31" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="88"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92">
+      <c r="B31" s="73"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77">
         <v>2</v>
       </c>
-      <c r="E31" s="92" t="s">
-        <v>165</v>
-      </c>
-      <c r="F31" s="88"/>
-      <c r="G31" s="89" t="s">
+      <c r="E31" s="77">
+        <v>1</v>
+      </c>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74" t="s">
         <v>133</v>
       </c>
-      <c r="H31" s="77" t="s">
+      <c r="H31" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="I31" s="77" t="s">
+      <c r="I31" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="J31" s="91"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="77">
+      <c r="J31" s="76"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="62">
         <v>12</v>
       </c>
-      <c r="M31" s="79">
+      <c r="M31" s="64">
         <f t="shared" si="3"/>
         <v>366</v>
       </c>
-      <c r="N31" s="79"/>
-      <c r="O31" s="93" t="str">
+      <c r="N31" s="64"/>
+      <c r="O31" s="78" t="str">
         <f>IF(J31="","",DATE(YEAR(J31)+1,MONTH(J31),DAY(J31)))</f>
         <v/>
       </c>
-      <c r="P31" s="81">
+      <c r="P31" s="66">
         <f t="shared" si="1"/>
         <v>731</v>
       </c>
-      <c r="Q31" s="81"/>
-      <c r="R31" s="94" t="str">
+      <c r="Q31" s="66"/>
+      <c r="R31" s="79" t="str">
         <f>IF(J31="","",DATE(YEAR(O31)+1,MONTH(O31),DAY(O31)))</f>
         <v/>
       </c>
-      <c r="S31" s="83">
+      <c r="S31" s="68">
         <f t="shared" si="2"/>
         <v>1096</v>
       </c>
-      <c r="T31" s="83"/>
-      <c r="U31" s="95" t="str">
+      <c r="T31" s="68"/>
+      <c r="U31" s="80" t="str">
         <f>IF(J31="","",DATE(YEAR(R31)+1,MONTH(R31),DAY(R31)))</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="87" t="s">
+    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88">
+      <c r="B32" s="73"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73">
         <v>7</v>
       </c>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="89" t="s">
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="H32" s="90" t="s">
+      <c r="H32" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="I32" s="77" t="s">
+      <c r="I32" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="J32" s="91">
+      <c r="J32" s="76">
         <v>44988</v>
       </c>
-      <c r="K32" s="78"/>
-      <c r="L32" s="77">
+      <c r="K32" s="63"/>
+      <c r="L32" s="62">
         <v>12</v>
       </c>
-      <c r="M32" s="79">
+      <c r="M32" s="64">
         <f t="shared" si="3"/>
         <v>45354</v>
       </c>
-      <c r="N32" s="79"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="81">
+      <c r="N32" s="64"/>
+      <c r="O32" s="78"/>
+      <c r="P32" s="66">
         <f t="shared" si="1"/>
         <v>45719</v>
       </c>
-      <c r="Q32" s="81"/>
-      <c r="R32" s="94"/>
-      <c r="S32" s="83">
+      <c r="Q32" s="66"/>
+      <c r="R32" s="79"/>
+      <c r="S32" s="68">
         <f t="shared" si="2"/>
         <v>46084</v>
       </c>
-      <c r="T32" s="83"/>
-      <c r="U32" s="95"/>
+      <c r="T32" s="68"/>
+      <c r="U32" s="80"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="hbLnOa1THPl6VRDDcvgevOenlotCxX/IUoR4M4tARoeLCyCe5vkrOb4wbxKSIu/QILfKuvYLESkbvVnliWua7Q==" saltValue="o7vtn2dhhnwjcOodTTVXpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
@@ -3593,142 +3565,142 @@
       <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="7"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="8" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="46" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="46" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="8" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="51">
+      <c r="E1" s="92">
         <v>2022</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53">
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="94">
         <v>2023</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="56">
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="96"/>
+      <c r="AC1" s="97">
         <v>2024</v>
       </c>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57"/>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="57"/>
-      <c r="AM1" s="57"/>
-      <c r="AN1" s="58"/>
-      <c r="AO1" s="59">
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="98"/>
+      <c r="AG1" s="98"/>
+      <c r="AH1" s="98"/>
+      <c r="AI1" s="98"/>
+      <c r="AJ1" s="98"/>
+      <c r="AK1" s="98"/>
+      <c r="AL1" s="98"/>
+      <c r="AM1" s="98"/>
+      <c r="AN1" s="99"/>
+      <c r="AO1" s="100">
         <v>2025</v>
       </c>
-      <c r="AP1" s="60"/>
-      <c r="AQ1" s="60"/>
-      <c r="AR1" s="60"/>
-      <c r="AS1" s="60"/>
-      <c r="AT1" s="60"/>
-      <c r="AU1" s="60"/>
-      <c r="AV1" s="60"/>
-      <c r="AW1" s="60"/>
-      <c r="AX1" s="60"/>
-      <c r="AY1" s="60"/>
-      <c r="AZ1" s="61"/>
-      <c r="BA1" s="62">
+      <c r="AP1" s="101"/>
+      <c r="AQ1" s="101"/>
+      <c r="AR1" s="101"/>
+      <c r="AS1" s="101"/>
+      <c r="AT1" s="101"/>
+      <c r="AU1" s="101"/>
+      <c r="AV1" s="101"/>
+      <c r="AW1" s="101"/>
+      <c r="AX1" s="101"/>
+      <c r="AY1" s="101"/>
+      <c r="AZ1" s="102"/>
+      <c r="BA1" s="103">
         <v>2026</v>
       </c>
-      <c r="BB1" s="62"/>
-      <c r="BC1" s="62"/>
-      <c r="BD1" s="62"/>
-      <c r="BE1" s="62"/>
-      <c r="BF1" s="62"/>
-      <c r="BG1" s="62"/>
-      <c r="BH1" s="62"/>
-      <c r="BI1" s="62"/>
-      <c r="BJ1" s="62"/>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="62"/>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+      <c r="BB1" s="103"/>
+      <c r="BC1" s="103"/>
+      <c r="BD1" s="103"/>
+      <c r="BE1" s="103"/>
+      <c r="BF1" s="103"/>
+      <c r="BG1" s="103"/>
+      <c r="BH1" s="103"/>
+      <c r="BI1" s="103"/>
+      <c r="BJ1" s="103"/>
+      <c r="BK1" s="103"/>
+      <c r="BL1" s="103"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>35</v>
       </c>
@@ -3922,7 +3894,7 @@
         <v>46357</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="str">
         <f>VLOOKUP(Clients!A4,Clients!A3:U12,1,FALSE)</f>
         <v xml:space="preserve">SOCIETE GENERALE FACTORING </v>
@@ -4180,7 +4152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="str">
         <f>VLOOKUP(Clients!A5,Clients!A4:U12,1,FALSE)</f>
         <v>DE WATOU</v>
@@ -4440,7 +4412,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="str">
         <f>VLOOKUP(Clients!A6,Clients!A5:U12,1,FALSE)</f>
         <v>CIBLEX</v>
@@ -4698,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="str">
         <f>VLOOKUP(Clients!A7,Clients!A6:U13,1,FALSE)</f>
         <v>AZUREVA LACANAU</v>
@@ -4956,7 +4928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="str">
         <f>VLOOKUP(Clients!A8,Clients!A7:U14,1,FALSE)</f>
         <v>INSTANTANE</v>
@@ -5214,7 +5186,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
         <f>VLOOKUP(Clients!A9,Clients!A8:U15,1,FALSE)</f>
         <v>CABINET DUBOST</v>
@@ -5472,7 +5444,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="str">
         <f>VLOOKUP(Clients!A10,Clients!A9:U16,1,FALSE)</f>
         <v xml:space="preserve">CEG Aqualia </v>
@@ -5730,7 +5702,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="str">
         <f>VLOOKUP(Clients!A11,Clients!A10:U17,1,FALSE)</f>
         <v>M ENERGIES</v>
@@ -5989,7 +5961,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="str">
         <f>VLOOKUP(Clients!A12,Clients!A11:U17,1,FALSE)</f>
         <v>AZUREVA LES VOSGES</v>
@@ -6249,7 +6221,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="str">
         <f>VLOOKUP(Clients!A13,Clients!A12:U18,1,FALSE)</f>
         <v>MAROQUINERIE AUGUSTE THOMAS</v>
@@ -6509,7 +6481,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="str">
         <f>VLOOKUP(Clients!A14,Clients!A13:U19,1,FALSE)</f>
         <v>MAROQUINERIE DE SAULIEU</v>
@@ -6769,7 +6741,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="str">
         <f>VLOOKUP(Clients!A15,Clients!A14:U20,1,FALSE)</f>
         <v>PGAM DI GENNARO</v>
@@ -7027,7 +6999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="str">
         <f>VLOOKUP(Clients!A16,Clients!A15:U21,1,FALSE)</f>
         <v>PGAM SOARES</v>
@@ -7285,7 +7257,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="str">
         <f>VLOOKUP(Clients!A17,Clients!A16:U22,1,FALSE)</f>
         <v>ARCONTROLS</v>
@@ -7543,7 +7515,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="str">
         <f>VLOOKUP(Clients!A18,Clients!A17:U23,1,FALSE)</f>
         <v>ARQUUS GUYANCOURT</v>
@@ -7801,7 +7773,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="str">
         <f>VLOOKUP(Clients!A19,Clients!A18:U23,1,FALSE)</f>
         <v>ARQUUS VERSAILLES</v>
@@ -8059,7 +8031,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="str">
         <f>VLOOKUP(Clients!A20,Clients!A19:U24,1,FALSE)</f>
         <v xml:space="preserve">AZUREVA ST CYPRIEN </v>
@@ -8077,7 +8049,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="str">
         <f>VLOOKUP(Clients!A21,Clients!A20:U25,1,FALSE)</f>
         <v>AZUREVA KARELLIS</v>
@@ -8095,7 +8067,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="str">
         <f>VLOOKUP(Clients!A22,Clients!A21:U26,1,FALSE)</f>
         <v xml:space="preserve">SEFAL ATOME </v>
@@ -8113,7 +8085,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="str">
         <f>VLOOKUP(Clients!A23,Clients!A22:U27,1,FALSE)</f>
         <v>NOVAXIA</v>
@@ -8131,7 +8103,7 @@
         <v>45364</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="str">
         <f>VLOOKUP(Clients!A25,Clients!A24:U30,1,FALSE)</f>
         <v>CENTRE TECHNIQUE COMMUNAUTAIRE SQY</v>
@@ -8149,7 +8121,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="str">
         <f>VLOOKUP(Clients!A24,Clients!A24:U29,1,FALSE)</f>
         <v xml:space="preserve">EPF MONTPELLIER </v>
@@ -8167,7 +8139,7 @@
         <v>45268</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="e">
         <f>VLOOKUP(Clients!#REF!,Clients!A23:U28,1,FALSE)</f>
         <v>#REF!</v>
@@ -8185,119 +8157,119 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
     </row>
   </sheetData>
@@ -8370,12 +8342,12 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -8383,7 +8355,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -8391,7 +8363,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -8412,7 +8384,7 @@
       <c r="V4" s="36"/>
       <c r="W4" s="37"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -8431,7 +8403,7 @@
       <c r="V5" s="39"/>
       <c r="W5" s="40"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -8456,7 +8428,7 @@
       <c r="V6" s="39"/>
       <c r="W6" s="40"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -8475,7 +8447,7 @@
       <c r="V7" s="39"/>
       <c r="W7" s="40"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>7</v>
       </c>
@@ -8493,7 +8465,7 @@
       <c r="V8" s="39"/>
       <c r="W8" s="40"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
         <v>8</v>
       </c>
@@ -8509,7 +8481,7 @@
       <c r="V9" s="39"/>
       <c r="W9" s="40"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>9</v>
       </c>
@@ -8527,7 +8499,7 @@
       <c r="V10" s="39"/>
       <c r="W10" s="40"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>10</v>
       </c>
@@ -8545,7 +8517,7 @@
       <c r="V11" s="39"/>
       <c r="W11" s="40"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M12" s="38"/>
       <c r="N12" s="39"/>
       <c r="O12" s="39"/>
@@ -8558,7 +8530,7 @@
       <c r="V12" s="39"/>
       <c r="W12" s="40"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M13" s="41" t="s">
         <v>96</v>
       </c>
@@ -8575,7 +8547,7 @@
       <c r="V13" s="39"/>
       <c r="W13" s="40"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M14" s="41" t="s">
         <v>97</v>
       </c>
@@ -8592,7 +8564,7 @@
       <c r="V14" s="39"/>
       <c r="W14" s="40"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M15" s="41" t="s">
         <v>98</v>
       </c>
@@ -8609,7 +8581,7 @@
       <c r="V15" s="39"/>
       <c r="W15" s="40"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M16" s="38"/>
       <c r="N16" s="39"/>
       <c r="O16" s="39"/>
@@ -8622,7 +8594,7 @@
       <c r="V16" s="39"/>
       <c r="W16" s="40"/>
     </row>
-    <row r="17" spans="13:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M17" s="38"/>
       <c r="N17" s="39"/>
       <c r="O17" s="39"/>
@@ -8635,7 +8607,7 @@
       <c r="V17" s="39"/>
       <c r="W17" s="40"/>
     </row>
-    <row r="18" spans="13:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M18" s="38" t="s">
         <v>94</v>
       </c>
@@ -8650,7 +8622,7 @@
       <c r="V18" s="39"/>
       <c r="W18" s="40"/>
     </row>
-    <row r="19" spans="13:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M19" s="38"/>
       <c r="N19" s="39"/>
       <c r="O19" s="39"/>
@@ -8663,7 +8635,7 @@
       <c r="V19" s="39"/>
       <c r="W19" s="40"/>
     </row>
-    <row r="20" spans="13:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M20" s="38" t="s">
         <v>95</v>
       </c>
@@ -8678,7 +8650,7 @@
       <c r="V20" s="39"/>
       <c r="W20" s="40"/>
     </row>
-    <row r="21" spans="13:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="13:23" x14ac:dyDescent="0.25">
       <c r="M21" s="42"/>
       <c r="N21" s="43"/>
       <c r="O21" s="43"/>
@@ -8706,13 +8678,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -8721,7 +8693,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -8729,7 +8701,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -8737,7 +8709,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -8745,7 +8717,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -8753,32 +8725,32 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -8797,6 +8769,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E948A9CE1FB2CE4C8AE9B70A9B9CE023" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb8a8860a1c4c91bbc706a6e17b12ecc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b78c6ca-c81e-4330-9bb3-0f577d436514" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33efc8288bb545af800450190bca8712" ns2:_="">
     <xsd:import namespace="6b78c6ca-c81e-4330-9bb3-0f577d436514"/>
@@ -8928,15 +8909,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8944,6 +8916,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E650D547-6807-4F22-A8C4-3B6D59729371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8961,14 +8941,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5F11FFB-EF31-444D-8074-B41CB27BA11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC99D9B8-395A-430E-937C-0EA8E9C71B29}">
   <ds:schemaRefs>

</xml_diff>